<commit_message>
bug fixes, code cleanup, and creation of presentation.R which creates a ppt file with comparative images of the nutrient modeling figures
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/countryCropVariety.xlsx
+++ b/data-raw/NutrientData/countryCropVariety.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/nutmod/data-raw/NutrientData/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9104F5-025E-184D-988A-1A6026FF8347}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="460" windowWidth="26440" windowHeight="15440" xr2:uid="{9AE6FF78-7D42-9B43-A8F0-3B48A49F20D8}"/>
+    <workbookView xWindow="-19880" yWindow="460" windowWidth="26440" windowHeight="15440" xr2:uid="{9AE6FF78-7D42-9B43-A8F0-3B48A49F20D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$FD$148</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="438">
   <si>
     <t>AFG</t>
   </si>
@@ -1160,9 +1161,6 @@
     <t>cmaiz</t>
   </si>
   <si>
-    <t>20014</t>
-  </si>
-  <si>
     <t>cmilk</t>
   </si>
   <si>
@@ -1337,23 +1335,20 @@
     <t>cwhea</t>
   </si>
   <si>
-    <t>20073</t>
-  </si>
-  <si>
     <t>cyams</t>
   </si>
   <si>
     <t>11601</t>
+  </si>
+  <si>
+    <t>20072</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1389,8 +1384,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1705,18 +1700,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A63CB7-DC64-3443-A6EF-3E2FE43CBA46}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:FD148"/>
+  <dimension ref="A1:FD63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DN62" sqref="DN62"/>
+      <selection pane="topRight" activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="7.83203125" customWidth="1"/>
     <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
@@ -1869,11 +1863,11 @@
     <col min="160" max="160" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:160">
+    <row r="1" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>316</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>317</v>
       </c>
       <c r="C1" t="s">
@@ -2351,7 +2345,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="2" spans="1:160" hidden="1">
+    <row r="2" spans="1:160" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>1</v>
       </c>
@@ -2827,7 +2821,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="3" spans="1:160" hidden="1">
+    <row r="3" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>318</v>
       </c>
@@ -2835,7 +2829,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="4" spans="1:160" hidden="1">
+    <row r="4" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>320</v>
       </c>
@@ -2843,7 +2837,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="5" spans="1:160" hidden="1">
+    <row r="5" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>322</v>
       </c>
@@ -2851,7 +2845,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="6" spans="1:160" hidden="1">
+    <row r="6" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>324</v>
       </c>
@@ -2859,7 +2853,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="7" spans="1:160" hidden="1">
+    <row r="7" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>326</v>
       </c>
@@ -2867,7 +2861,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="8" spans="1:160" hidden="1">
+    <row r="8" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>328</v>
       </c>
@@ -2875,7 +2869,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="9" spans="1:160" hidden="1">
+    <row r="9" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>330</v>
       </c>
@@ -2883,7 +2877,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="10" spans="1:160" hidden="1">
+    <row r="10" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>332</v>
       </c>
@@ -2891,7 +2885,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="11" spans="1:160" hidden="1">
+    <row r="11" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>334</v>
       </c>
@@ -2899,7 +2893,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="12" spans="1:160" hidden="1">
+    <row r="12" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>336</v>
       </c>
@@ -2907,7 +2901,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="13" spans="1:160" hidden="1">
+    <row r="13" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>338</v>
       </c>
@@ -2915,7 +2909,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="14" spans="1:160" hidden="1">
+    <row r="14" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>340</v>
       </c>
@@ -2923,7 +2917,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="15" spans="1:160" hidden="1">
+    <row r="15" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>342</v>
       </c>
@@ -2931,7 +2925,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="16" spans="1:160" hidden="1">
+    <row r="16" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>344</v>
       </c>
@@ -2939,7 +2933,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="17" spans="1:160" hidden="1">
+    <row r="17" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>346</v>
       </c>
@@ -2947,7 +2941,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="18" spans="1:160" hidden="1">
+    <row r="18" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>348</v>
       </c>
@@ -2955,7 +2949,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="19" spans="1:160" hidden="1">
+    <row r="19" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>350</v>
       </c>
@@ -2963,7 +2957,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="20" spans="1:160" hidden="1">
+    <row r="20" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>352</v>
       </c>
@@ -2971,7 +2965,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="21" spans="1:160" hidden="1">
+    <row r="21" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>354</v>
       </c>
@@ -2979,7 +2973,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="22" spans="1:160" hidden="1">
+    <row r="22" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>356</v>
       </c>
@@ -2987,7 +2981,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="23" spans="1:160" hidden="1">
+    <row r="23" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>358</v>
       </c>
@@ -2995,7 +2989,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="24" spans="1:160" hidden="1">
+    <row r="24" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>360</v>
       </c>
@@ -3003,7 +2997,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="25" spans="1:160" hidden="1">
+    <row r="25" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>362</v>
       </c>
@@ -3011,7 +3005,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="26" spans="1:160" hidden="1">
+    <row r="26" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>364</v>
       </c>
@@ -3019,7 +3013,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="27" spans="1:160" hidden="1">
+    <row r="27" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>366</v>
       </c>
@@ -3027,7 +3021,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="28" spans="1:160" hidden="1">
+    <row r="28" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>368</v>
       </c>
@@ -3035,7 +3029,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="29" spans="1:160" hidden="1">
+    <row r="29" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>370</v>
       </c>
@@ -3043,7 +3037,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="30" spans="1:160" hidden="1">
+    <row r="30" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>372</v>
       </c>
@@ -3051,7 +3045,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="31" spans="1:160" hidden="1">
+    <row r="31" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>374</v>
       </c>
@@ -3059,12 +3053,12 @@
         <v>375</v>
       </c>
     </row>
-    <row r="32" spans="1:160">
+    <row r="32" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>376</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>377</v>
+      <c r="B32" s="1">
+        <v>20020</v>
       </c>
       <c r="AT32">
         <v>20314</v>
@@ -3103,115 +3097,115 @@
         <v>20314</v>
       </c>
     </row>
-    <row r="33" spans="1:155" hidden="1">
+    <row r="33" spans="1:155" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>377</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="B33" s="1" t="s">
+    </row>
+    <row r="34" spans="1:155" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="34" spans="1:155" hidden="1">
-      <c r="A34" t="s">
+      <c r="B34" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B34" s="1" t="s">
+    </row>
+    <row r="35" spans="1:155" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="35" spans="1:155" hidden="1">
-      <c r="A35" t="s">
+      <c r="B35" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="B35" s="1" t="s">
+    </row>
+    <row r="36" spans="1:155" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="36" spans="1:155" hidden="1">
-      <c r="A36" t="s">
+      <c r="B36" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B36" s="1" t="s">
+    </row>
+    <row r="37" spans="1:155" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="37" spans="1:155" hidden="1">
-      <c r="A37" t="s">
+      <c r="B37" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="B37" s="1" t="s">
+    </row>
+    <row r="38" spans="1:155" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="38" spans="1:155" hidden="1">
-      <c r="A38" t="s">
+      <c r="B38" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="B38" s="1" t="s">
+    </row>
+    <row r="39" spans="1:155" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="39" spans="1:155" hidden="1">
-      <c r="A39" t="s">
+      <c r="B39" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="B39" s="1" t="s">
+    </row>
+    <row r="40" spans="1:155" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="40" spans="1:155" hidden="1">
-      <c r="A40" t="s">
+      <c r="B40" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="B40" s="1" t="s">
+    </row>
+    <row r="41" spans="1:155" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="41" spans="1:155" hidden="1">
-      <c r="A41" t="s">
+      <c r="B41" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="B41" s="1" t="s">
+    </row>
+    <row r="42" spans="1:155" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="42" spans="1:155" hidden="1">
-      <c r="A42" t="s">
+      <c r="B42" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="B42" s="1" t="s">
+    </row>
+    <row r="43" spans="1:155" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="43" spans="1:155" hidden="1">
-      <c r="A43" t="s">
+      <c r="B43" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="B43" s="1" t="s">
+    </row>
+    <row r="44" spans="1:155" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="44" spans="1:155" hidden="1">
-      <c r="A44" t="s">
+      <c r="B44" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="B44" s="1" t="s">
+    </row>
+    <row r="45" spans="1:155" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="45" spans="1:155" hidden="1">
-      <c r="A45" t="s">
+      <c r="B45" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="B45" s="1" t="s">
+    </row>
+    <row r="46" spans="1:155" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="46" spans="1:155">
-      <c r="A46" t="s">
-        <v>404</v>
-      </c>
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>20444</v>
       </c>
       <c r="N46">
@@ -3263,132 +3257,132 @@
         <v>20450</v>
       </c>
     </row>
-    <row r="47" spans="1:155" hidden="1">
+    <row r="47" spans="1:155" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>404</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="B47" s="1" t="s">
+    </row>
+    <row r="48" spans="1:155" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="48" spans="1:155" hidden="1">
-      <c r="A48" t="s">
+      <c r="B48" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="B48" s="1" t="s">
+    </row>
+    <row r="49" spans="1:118" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="49" spans="1:118" hidden="1">
-      <c r="A49" t="s">
+      <c r="B49" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="B49" s="1" t="s">
+    </row>
+    <row r="50" spans="1:118" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="50" spans="1:118" hidden="1">
-      <c r="A50" t="s">
+      <c r="B50" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="B50" s="1" t="s">
+    </row>
+    <row r="51" spans="1:118" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="51" spans="1:118" hidden="1">
-      <c r="A51" t="s">
+      <c r="B51" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="B51" s="1" t="s">
+    </row>
+    <row r="52" spans="1:118" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="52" spans="1:118" hidden="1">
-      <c r="A52" t="s">
+      <c r="B52" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="B52" s="1" t="s">
+    </row>
+    <row r="53" spans="1:118" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="53" spans="1:118" hidden="1">
-      <c r="A53" t="s">
+      <c r="B53" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="B53" s="1" t="s">
+    </row>
+    <row r="54" spans="1:118" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="54" spans="1:118" hidden="1">
-      <c r="A54" t="s">
+      <c r="B54" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="B54" s="1" t="s">
+    </row>
+    <row r="55" spans="1:118" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="55" spans="1:118" hidden="1">
-      <c r="A55" t="s">
+      <c r="B55" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="B55" s="1" t="s">
+    </row>
+    <row r="56" spans="1:118" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="56" spans="1:118" hidden="1">
-      <c r="A56" t="s">
+      <c r="B56" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="B56" s="1" t="s">
+    </row>
+    <row r="57" spans="1:118" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="57" spans="1:118" hidden="1">
-      <c r="A57" t="s">
+      <c r="B57" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="B57" s="1" t="s">
+    </row>
+    <row r="58" spans="1:118" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="58" spans="1:118" hidden="1">
-      <c r="A58" t="s">
+      <c r="B58" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="B58" s="1" t="s">
+    </row>
+    <row r="59" spans="1:118" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="59" spans="1:118" hidden="1">
-      <c r="A59" t="s">
+      <c r="B59" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="B59" s="1" t="s">
+    </row>
+    <row r="60" spans="1:118" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="60" spans="1:118" hidden="1">
-      <c r="A60" t="s">
+      <c r="B60" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="B60" s="1" t="s">
+    </row>
+    <row r="61" spans="1:118" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="61" spans="1:118" hidden="1">
-      <c r="A61" t="s">
+      <c r="B61" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="B61" s="1" t="s">
+    </row>
+    <row r="62" spans="1:118" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="62" spans="1:118">
-      <c r="A62" t="s">
-        <v>435</v>
-      </c>
       <c r="B62" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="AA62">
         <v>20075</v>
@@ -3409,109 +3403,15 @@
         <v>20074</v>
       </c>
     </row>
-    <row r="63" spans="1:118" hidden="1">
+    <row r="63" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="64" spans="1:118" hidden="1"/>
-    <row r="65" hidden="1"/>
-    <row r="66" hidden="1"/>
-    <row r="67" hidden="1"/>
-    <row r="68" hidden="1"/>
-    <row r="69" hidden="1"/>
-    <row r="70" hidden="1"/>
-    <row r="71" hidden="1"/>
-    <row r="72" hidden="1"/>
-    <row r="73" hidden="1"/>
-    <row r="74" hidden="1"/>
-    <row r="75" hidden="1"/>
-    <row r="76" hidden="1"/>
-    <row r="77" hidden="1"/>
-    <row r="78" hidden="1"/>
-    <row r="79" hidden="1"/>
-    <row r="80" hidden="1"/>
-    <row r="81" hidden="1"/>
-    <row r="82" hidden="1"/>
-    <row r="83" hidden="1"/>
-    <row r="84" hidden="1"/>
-    <row r="85" hidden="1"/>
-    <row r="86" hidden="1"/>
-    <row r="87" hidden="1"/>
-    <row r="88" hidden="1"/>
-    <row r="89" hidden="1"/>
-    <row r="90" hidden="1"/>
-    <row r="91" hidden="1"/>
-    <row r="92" hidden="1"/>
-    <row r="93" hidden="1"/>
-    <row r="94" hidden="1"/>
-    <row r="95" hidden="1"/>
-    <row r="96" hidden="1"/>
-    <row r="97" hidden="1"/>
-    <row r="98" hidden="1"/>
-    <row r="99" hidden="1"/>
-    <row r="100" hidden="1"/>
-    <row r="101" hidden="1"/>
-    <row r="102" hidden="1"/>
-    <row r="103" hidden="1"/>
-    <row r="104" hidden="1"/>
-    <row r="105" hidden="1"/>
-    <row r="106" hidden="1"/>
-    <row r="107" hidden="1"/>
-    <row r="108" hidden="1"/>
-    <row r="109" hidden="1"/>
-    <row r="110" hidden="1"/>
-    <row r="111" hidden="1"/>
-    <row r="112" hidden="1"/>
-    <row r="113" hidden="1"/>
-    <row r="114" hidden="1"/>
-    <row r="115" hidden="1"/>
-    <row r="116" hidden="1"/>
-    <row r="117" hidden="1"/>
-    <row r="118" hidden="1"/>
-    <row r="119" hidden="1"/>
-    <row r="120" hidden="1"/>
-    <row r="121" hidden="1"/>
-    <row r="122" hidden="1"/>
-    <row r="123" hidden="1"/>
-    <row r="124" hidden="1"/>
-    <row r="125" hidden="1"/>
-    <row r="126" hidden="1"/>
-    <row r="127" hidden="1"/>
-    <row r="128" hidden="1"/>
-    <row r="129" hidden="1"/>
-    <row r="130" hidden="1"/>
-    <row r="131" hidden="1"/>
-    <row r="132" hidden="1"/>
-    <row r="133" hidden="1"/>
-    <row r="134" hidden="1"/>
-    <row r="135" hidden="1"/>
-    <row r="136" hidden="1"/>
-    <row r="137" hidden="1"/>
-    <row r="138" hidden="1"/>
-    <row r="139" hidden="1"/>
-    <row r="140" hidden="1"/>
-    <row r="141" hidden="1"/>
-    <row r="142" hidden="1"/>
-    <row r="143" hidden="1"/>
-    <row r="144" hidden="1"/>
-    <row r="145" hidden="1"/>
-    <row r="146" hidden="1"/>
-    <row r="147" hidden="1"/>
-    <row r="148" hidden="1"/>
+        <v>436</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:FD148" xr:uid="{A425F7E0-F9B4-D841-9279-7B3C96A92AE6}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="cmaiz"/>
-        <filter val="crice"/>
-        <filter val="cwhea"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>